<commit_message>
FIX - stationary workouts with altitude but no distance data
workouts that had altitude, but no distance data caused trouble with
altitude smoothing. This fix checks for this before trying to smooth
altitude
</commit_message>
<xml_diff>
--- a/misc/StraTistiX Test Workouts Links.xlsx
+++ b/misc/StraTistiX Test Workouts Links.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="138">
   <si>
     <t xml:space="preserve">Bike:                                         </t>
   </si>
@@ -418,6 +418,18 @@
   </si>
   <si>
     <t xml:space="preserve">(GPS)            </t>
+  </si>
+  <si>
+    <t>(HR, temperature, altitude)</t>
+  </si>
+  <si>
+    <t>* altitude, but no distance</t>
+  </si>
+  <si>
+    <t>https://www.strava.com/activities/492714906</t>
+  </si>
+  <si>
+    <t>export CSV doesn't work!!!</t>
   </si>
 </sst>
 </file>
@@ -784,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,7 +1265,7 @@
         <v>99</v>
       </c>
       <c r="F27" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1461,20 +1473,20 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>3</v>
+      <c r="A40" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="C40" t="s">
         <v>61</v>
       </c>
       <c r="D40" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="E40" t="s">
         <v>83</v>
       </c>
       <c r="F40" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2513,9 +2525,10 @@
     <hyperlink ref="A88" r:id="rId40"/>
     <hyperlink ref="A96" r:id="rId41"/>
     <hyperlink ref="A101" r:id="rId42"/>
+    <hyperlink ref="A40" r:id="rId43"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId43"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId44"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
misc testing excel files "cleanup"
</commit_message>
<xml_diff>
--- a/misc/StraTistiX Test Workouts Links.xlsx
+++ b/misc/StraTistiX Test Workouts Links.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="138">
   <si>
     <t xml:space="preserve">Bike:                                         </t>
   </si>
@@ -162,9 +162,6 @@
     <t xml:space="preserve">https://www.strava.com/activities/83623294    </t>
   </si>
   <si>
-    <t xml:space="preserve">* a bit hilly *                               </t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.strava.com/activities/83625038    </t>
   </si>
   <si>
@@ -309,9 +306,6 @@
     <t xml:space="preserve">mountainous   My Riđ                  </t>
   </si>
   <si>
-    <t xml:space="preserve">mountainous   Marcel Wyss TdF 12      </t>
-  </si>
-  <si>
     <t xml:space="preserve">mountainous   My                      </t>
   </si>
   <si>
@@ -336,9 +330,6 @@
     <t xml:space="preserve">mostly flat   My                      </t>
   </si>
   <si>
-    <t xml:space="preserve">mostly flat   My nabrežje             </t>
-  </si>
-  <si>
     <t xml:space="preserve">a bit hilly   My park, 3r             </t>
   </si>
   <si>
@@ -372,9 +363,6 @@
     <t xml:space="preserve">mostly flat    My LJ                  </t>
   </si>
   <si>
-    <t xml:space="preserve">hilly (could also be a bit hilly) my  </t>
-  </si>
-  <si>
     <t xml:space="preserve">hilly          My trikotna            </t>
   </si>
   <si>
@@ -430,6 +418,18 @@
   </si>
   <si>
     <t>export CSV doesn't work!!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a bit hilly my  </t>
+  </si>
+  <si>
+    <t>* downhill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flat   My nabrežje             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">very hilly   Marcel Wyss TdF 12      </t>
   </si>
 </sst>
 </file>
@@ -794,10 +794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F104"/>
+  <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,19 +811,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -831,16 +831,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -848,16 +848,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -865,16 +865,16 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -882,16 +882,16 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -899,16 +899,16 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F6" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -916,16 +916,16 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -933,16 +933,16 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F8" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -950,16 +950,16 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F9" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -967,16 +967,16 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F10" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -984,16 +984,16 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F11" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1001,16 +1001,16 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F12" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1018,16 +1018,16 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F13" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1035,16 +1035,16 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F14" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1052,16 +1052,16 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F15" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1069,16 +1069,16 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1086,16 +1086,16 @@
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F17" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1103,16 +1103,16 @@
         <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F18" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1120,16 +1120,16 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F19" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1137,16 +1137,16 @@
         <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1154,67 +1154,67 @@
         <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F21" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>3</v>
+      <c r="A22" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C22" t="s">
         <v>61</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E22" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="F22" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>15</v>
+      <c r="A23" t="s">
+        <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E23" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="F23" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D24" t="s">
         <v>72</v>
       </c>
       <c r="E24" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F24" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1222,16 +1222,16 @@
         <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E25" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F25" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1239,16 +1239,16 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F26" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1256,16 +1256,16 @@
         <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F27" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1273,16 +1273,16 @@
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F28" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1290,16 +1290,16 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F29" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1307,16 +1307,16 @@
         <v>19</v>
       </c>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F30" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1324,16 +1324,16 @@
         <v>20</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1341,16 +1341,16 @@
         <v>21</v>
       </c>
       <c r="C32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E32" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F32" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1358,16 +1358,16 @@
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F33" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1375,16 +1375,16 @@
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F34" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1392,16 +1392,16 @@
         <v>22</v>
       </c>
       <c r="C35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F35" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1409,16 +1409,16 @@
         <v>23</v>
       </c>
       <c r="C36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E36" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F36" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1426,16 +1426,16 @@
         <v>24</v>
       </c>
       <c r="C37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E37" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F37" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1443,16 +1443,16 @@
         <v>25</v>
       </c>
       <c r="C38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E38" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F38" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1460,33 +1460,33 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E39" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F39" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D40" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F40" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1494,16 +1494,16 @@
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F41" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1511,16 +1511,16 @@
         <v>26</v>
       </c>
       <c r="C42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F42" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1528,16 +1528,16 @@
         <v>27</v>
       </c>
       <c r="C43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E43" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F43" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1545,33 +1545,33 @@
         <v>28</v>
       </c>
       <c r="C44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E44" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F44" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E45" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F45" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1579,16 +1579,16 @@
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F46" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1596,16 +1596,16 @@
         <v>29</v>
       </c>
       <c r="C47" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F47" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1613,16 +1613,16 @@
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E48" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F48" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1630,84 +1630,84 @@
         <v>30</v>
       </c>
       <c r="C49" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E49" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F49" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>3</v>
+      <c r="A50" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="C50" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D50" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E50" t="s">
-        <v>83</v>
+        <v>136</v>
       </c>
       <c r="F50" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>31</v>
+      <c r="A51" t="s">
+        <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D51" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E51" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="F51" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D52" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E52" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F52" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E53" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F53" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -1715,16 +1715,16 @@
         <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F54" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1732,16 +1732,16 @@
         <v>34</v>
       </c>
       <c r="C55" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E55" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F55" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -1749,16 +1749,16 @@
         <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D56" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E56" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F56" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -1766,16 +1766,16 @@
         <v>35</v>
       </c>
       <c r="C57" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D57" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E57" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F57" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -1783,16 +1783,16 @@
         <v>36</v>
       </c>
       <c r="C58" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D58" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E58" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F58" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -1800,16 +1800,16 @@
         <v>37</v>
       </c>
       <c r="C59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D59" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E59" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F59" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -1817,16 +1817,16 @@
         <v>38</v>
       </c>
       <c r="C60" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D60" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E60" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F60" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -1834,16 +1834,16 @@
         <v>3</v>
       </c>
       <c r="C61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D61" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E61" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F61" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -1851,16 +1851,16 @@
         <v>39</v>
       </c>
       <c r="C62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D62" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E62" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F62" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -1868,16 +1868,16 @@
         <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D63" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E63" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F63" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1885,16 +1885,16 @@
         <v>40</v>
       </c>
       <c r="C64" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D64" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E64" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F64" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1902,16 +1902,16 @@
         <v>41</v>
       </c>
       <c r="C65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D65" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E65" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F65" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1919,16 +1919,16 @@
         <v>3</v>
       </c>
       <c r="C66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D66" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E66" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F66" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -1936,16 +1936,16 @@
         <v>42</v>
       </c>
       <c r="C67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E67" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F67" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -1953,16 +1953,16 @@
         <v>3</v>
       </c>
       <c r="C68" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E68" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F68" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -1970,16 +1970,16 @@
         <v>3</v>
       </c>
       <c r="C69" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D69" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E69" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F69" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -1987,16 +1987,16 @@
         <v>43</v>
       </c>
       <c r="C70" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E70" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F70" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2004,16 +2004,16 @@
         <v>1</v>
       </c>
       <c r="C71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D71" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E71" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F71" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2021,16 +2021,16 @@
         <v>44</v>
       </c>
       <c r="C72" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E72" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F72" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2038,16 +2038,16 @@
         <v>3</v>
       </c>
       <c r="C73" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D73" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F73" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2055,16 +2055,16 @@
         <v>45</v>
       </c>
       <c r="C74" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D74" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E74" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F74" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2072,16 +2072,16 @@
         <v>3</v>
       </c>
       <c r="C75" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D75" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E75" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F75" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2089,16 +2089,16 @@
         <v>46</v>
       </c>
       <c r="C76" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D76" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E76" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F76" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2106,16 +2106,16 @@
         <v>3</v>
       </c>
       <c r="C77" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D77" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E77" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F77" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2123,16 +2123,16 @@
         <v>47</v>
       </c>
       <c r="C78" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D78" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E78" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F78" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2140,33 +2140,33 @@
         <v>3</v>
       </c>
       <c r="C79" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D79" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E79" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F79" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="A80" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C80" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D80" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="E80" t="s">
-        <v>83</v>
+        <v>134</v>
       </c>
       <c r="F80" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2174,16 +2174,16 @@
         <v>3</v>
       </c>
       <c r="C81" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D81" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E81" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F81" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2191,16 +2191,16 @@
         <v>49</v>
       </c>
       <c r="C82" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D82" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="E82" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F82" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2208,33 +2208,33 @@
         <v>3</v>
       </c>
       <c r="C83" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D83" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E83" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F83" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+      <c r="A84" t="s">
         <v>50</v>
       </c>
       <c r="C84" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D84" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E84" t="s">
-        <v>119</v>
+        <v>82</v>
       </c>
       <c r="F84" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2242,33 +2242,33 @@
         <v>3</v>
       </c>
       <c r="C85" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D85" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E85" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F85" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="A86" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C86" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D86" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E86" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="F86" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2276,33 +2276,30 @@
         <v>3</v>
       </c>
       <c r="C87" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D87" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E87" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F87" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+      <c r="A88" t="s">
         <v>52</v>
       </c>
       <c r="C88" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D88" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E88" t="s">
-        <v>120</v>
-      </c>
-      <c r="F88" t="s">
-        <v>124</v>
+        <v>82</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2310,30 +2307,24 @@
         <v>3</v>
       </c>
       <c r="C89" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D89" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E89" t="s">
-        <v>83</v>
-      </c>
-      <c r="F89" t="s">
-        <v>124</v>
+        <v>82</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="C90" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D90" t="s">
-        <v>69</v>
-      </c>
-      <c r="E90" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2341,144 +2332,119 @@
         <v>3</v>
       </c>
       <c r="C91" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D91" t="s">
-        <v>69</v>
-      </c>
-      <c r="E91" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="C92" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D92" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="C93" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D93" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>54</v>
+      <c r="A94" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="C94" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D94" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="C95" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D95" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>56</v>
+      <c r="A96" t="s">
+        <v>3</v>
       </c>
       <c r="C96" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D96" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="C97" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D97" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="C98" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D98" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="A99" s="1" t="s">
         <v>57</v>
       </c>
       <c r="C99" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D99" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="C100" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D100" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="C101" t="s">
-        <v>61</v>
-      </c>
-      <c r="D101" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>3</v>
-      </c>
       <c r="C102" t="s">
-        <v>61</v>
-      </c>
-      <c r="D102" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C103" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C104" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2495,8 +2461,8 @@
     <hyperlink ref="A18" r:id="rId10"/>
     <hyperlink ref="A20" r:id="rId11"/>
     <hyperlink ref="A21" r:id="rId12"/>
-    <hyperlink ref="A23" r:id="rId13"/>
-    <hyperlink ref="A24" r:id="rId14"/>
+    <hyperlink ref="A24" r:id="rId13"/>
+    <hyperlink ref="A22" r:id="rId14"/>
     <hyperlink ref="A25" r:id="rId15"/>
     <hyperlink ref="A27" r:id="rId16"/>
     <hyperlink ref="A32" r:id="rId17"/>
@@ -2506,9 +2472,9 @@
     <hyperlink ref="A45" r:id="rId21"/>
     <hyperlink ref="A47" r:id="rId22"/>
     <hyperlink ref="A49" r:id="rId23"/>
-    <hyperlink ref="A51" r:id="rId24"/>
-    <hyperlink ref="A52" r:id="rId25"/>
-    <hyperlink ref="A53" r:id="rId26"/>
+    <hyperlink ref="A52" r:id="rId24"/>
+    <hyperlink ref="A53" r:id="rId25"/>
+    <hyperlink ref="A50" r:id="rId26"/>
     <hyperlink ref="A55" r:id="rId27"/>
     <hyperlink ref="A57" r:id="rId28"/>
     <hyperlink ref="A58" r:id="rId29"/>
@@ -2520,11 +2486,11 @@
     <hyperlink ref="A72" r:id="rId35"/>
     <hyperlink ref="A76" r:id="rId36"/>
     <hyperlink ref="A78" r:id="rId37"/>
-    <hyperlink ref="A82" r:id="rId38"/>
-    <hyperlink ref="A84" r:id="rId39"/>
-    <hyperlink ref="A88" r:id="rId40"/>
-    <hyperlink ref="A96" r:id="rId41"/>
-    <hyperlink ref="A101" r:id="rId42"/>
+    <hyperlink ref="A80" r:id="rId38"/>
+    <hyperlink ref="A82" r:id="rId39"/>
+    <hyperlink ref="A86" r:id="rId40"/>
+    <hyperlink ref="A94" r:id="rId41"/>
+    <hyperlink ref="A99" r:id="rId42"/>
     <hyperlink ref="A40" r:id="rId43"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>